<commit_message>
Add Register Tests and more Tests for SignInTests.
</commit_message>
<xml_diff>
--- a/new360TestCasesforAutomation.xlsx
+++ b/new360TestCasesforAutomation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sing IN with Email" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
-  <si>
-    <t>Ticket id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>Test results</t>
   </si>
@@ -68,9 +65,6 @@
   </si>
   <si>
     <t>failed</t>
-  </si>
-  <si>
-    <t>Validation mesage  - "Invalid login or password"</t>
   </si>
   <si>
     <t>Can_not_do_more_than_five_only_five_attempts _with_wrong_login</t>
@@ -201,9 +195,6 @@
     <t>Can_not_signUp_with_not_matched_password_and_conformation_password</t>
   </si>
   <si>
-    <t>Can_not_sign_in_with_empty_data</t>
-  </si>
-  <si>
     <t>To Automate</t>
   </si>
   <si>
@@ -214,13 +205,81 @@
   </si>
   <si>
     <t>Can_Sign_In_with_valid_email_and_password()</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Can_not_sign_in_with_empty_empty_data</t>
+  </si>
+  <si>
+    <t>15/05/2016</t>
+  </si>
+  <si>
+    <t>Can_not_sign_in_with_empty_data()</t>
+  </si>
+  <si>
+    <t>Can_not_sign_in_with_non_registered_email()</t>
+  </si>
+  <si>
+    <r>
+      <t>Validation message - "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>This value is required.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Validation mesage  - "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Invalid login or password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Can_not_sign_in_with_registered_email_but_wrong_password()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,8 +314,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,14 +358,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCFF33"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFEFEFEF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFF33"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -321,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -352,7 +421,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -673,30 +747,30 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -709,167 +783,195 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="B6">
-        <v>3</v>
-      </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30">
+      <c r="B9" s="16">
+        <v>3</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
         <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
         <v>16</v>
       </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="C16" t="s">
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="C22" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
-      <c r="C18" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30">
-      <c r="B19">
+    <row r="23" spans="2:7" ht="30">
+      <c r="B23">
         <v>10</v>
       </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" t="s">
-        <v>41</v>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -882,150 +984,156 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="88.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
     <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="C3">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
+      <c r="B6" s="16">
+        <v>2</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="D4" t="s">
+    <row r="7" spans="1:7">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45">
+      <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
         <v>15</v>
       </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="45">
-      <c r="D10" s="5" t="s">
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="19" spans="2:7">
+      <c r="C19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="D15" t="s">
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="3:5">
-      <c r="D19" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5">
-      <c r="C20">
-        <v>6</v>
-      </c>
       <c r="D20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new scenario Can_not_signUp_with_not_matched_password_and_conformation_password()
</commit_message>
<xml_diff>
--- a/new360TestCasesforAutomation.xlsx
+++ b/new360TestCasesforAutomation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sing IN with Email" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
   <si>
     <t>Test results</t>
   </si>
@@ -728,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1081,6 +1081,12 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
+      <c r="F9" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="45">
       <c r="C10" s="5" t="s">

</xml_diff>